<commit_message>
worked on ecoabric projects.
</commit_message>
<xml_diff>
--- a/Eco shelter project/logger data.xlsx
+++ b/Eco shelter project/logger data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12130" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12130" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Trial 1" sheetId="1" r:id="rId1"/>
@@ -17,6 +17,7 @@
     <sheet name="Trial 3" sheetId="3" r:id="rId3"/>
     <sheet name="trial 4" sheetId="4" r:id="rId4"/>
     <sheet name="trial 5" sheetId="5" r:id="rId5"/>
+    <sheet name="trial 6" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="25">
   <si>
     <t>microsite</t>
   </si>
@@ -97,6 +98,12 @@
   </si>
   <si>
     <t>larrea 1</t>
+  </si>
+  <si>
+    <t>open1</t>
+  </si>
+  <si>
+    <t>L1</t>
   </si>
 </sst>
 </file>
@@ -875,6 +882,98 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2">
+        <v>20881733</v>
+      </c>
+      <c r="C2">
+        <v>15489</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3">
+        <v>20881753</v>
+      </c>
+      <c r="C3">
+        <v>15512</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4">
+        <v>15406</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <v>20884543</v>
+      </c>
+      <c r="C5">
+        <v>15531</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>20881725</v>
+      </c>
+      <c r="C6">
+        <v>15402</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>20881726</v>
+      </c>
+      <c r="C7">
+        <v>15491</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
@@ -897,18 +996,18 @@
         <v>21</v>
       </c>
       <c r="B2">
-        <v>20881733</v>
+        <v>20881725</v>
       </c>
       <c r="C2">
-        <v>15489</v>
+        <v>15406</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="B3">
-        <v>20881753</v>
+        <v>20881726</v>
       </c>
       <c r="C3">
         <v>15512</v>
@@ -916,32 +1015,32 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C4">
-        <v>15406</v>
+        <v>15289</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B5">
         <v>20884543</v>
       </c>
       <c r="C5">
-        <v>15531</v>
+        <v>15491</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B6">
-        <v>20881725</v>
+        <v>20881753</v>
       </c>
       <c r="C6">
         <v>15402</v>
@@ -949,13 +1048,13 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B7">
-        <v>20881726</v>
+        <v>20881733</v>
       </c>
       <c r="C7">
-        <v>155491</v>
+        <v>15531</v>
       </c>
     </row>
   </sheetData>

</xml_diff>